<commit_message>
ListForExectution ProductSummery hide/show test
</commit_message>
<xml_diff>
--- a/testdata/listForExecution.xlsx
+++ b/testdata/listForExecution.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>TestName</t>
   </si>
@@ -123,6 +123,12 @@
   </si>
   <si>
     <t>C70772</t>
+  </si>
+  <si>
+    <t>Product_Summary-Hide/Show_account_on_Product_List_[WEB]_1</t>
+  </si>
+  <si>
+    <t>C70773</t>
   </si>
 </sst>
 </file>
@@ -1081,10 +1087,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1372,8 +1378,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F13" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F14" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Aleksin test Dashboard General-Dashboard-Page_overview
</commit_message>
<xml_diff>
--- a/testdata/listForExecution.xlsx
+++ b/testdata/listForExecution.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="35">
   <si>
     <t>TestName</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>C70773</t>
+  </si>
+  <si>
+    <t>General-Dashboard-Page_overview_[WEB]</t>
+  </si>
+  <si>
+    <t>C70774</t>
   </si>
 </sst>
 </file>
@@ -1087,10 +1093,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1398,8 +1404,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F14" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F15" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dodat Foreign test za Download
</commit_message>
<xml_diff>
--- a/testdata/listForExecution.xlsx
+++ b/testdata/listForExecution.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="47">
   <si>
     <t>TestName</t>
   </si>
@@ -159,6 +159,18 @@
   </si>
   <si>
     <t>C70778</t>
+  </si>
+  <si>
+    <t>Foreign_Current_Accounts-Transactions-Filter_By_Type_[WEB]</t>
+  </si>
+  <si>
+    <t>C70779</t>
+  </si>
+  <si>
+    <t>Current_Foreign_Accounts-Transactions-Download_option_[WEB]</t>
+  </si>
+  <si>
+    <t>C70780</t>
   </si>
 </sst>
 </file>
@@ -1111,10 +1123,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1522,8 +1534,48 @@
         <v>11</v>
       </c>
     </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F19" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F20" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dodavanje testova u listForExecution
</commit_message>
<xml_diff>
--- a/testdata/listForExecution.xlsx
+++ b/testdata/listForExecution.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="78">
   <si>
     <t>TestName</t>
   </si>
@@ -240,6 +240,30 @@
   </si>
   <si>
     <t>C70791</t>
+  </si>
+  <si>
+    <t>Product_Summary-Credit_Card_List_[WEB]_1</t>
+  </si>
+  <si>
+    <t>C70792</t>
+  </si>
+  <si>
+    <t>Manage_Products-Favorite_account_[WEB]</t>
+  </si>
+  <si>
+    <t>C70793</t>
+  </si>
+  <si>
+    <t>Manage_Products-Favorite_account-Removal_of_the_favorite_account_[WEB]</t>
+  </si>
+  <si>
+    <t>C70794</t>
+  </si>
+  <si>
+    <t>Term_Deposits_Lists_[WEB]</t>
+  </si>
+  <si>
+    <t>C70795</t>
   </si>
 </sst>
 </file>
@@ -1192,10 +1216,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1903,8 +1927,88 @@
         <v>11</v>
       </c>
     </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F33" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F35" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prosli svi testovi 20 min - 16.12.25.
</commit_message>
<xml_diff>
--- a/testdata/listForExecution.xlsx
+++ b/testdata/listForExecution.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="106">
   <si>
     <t>TestName</t>
   </si>
@@ -110,238 +110,244 @@
     <t>C70771</t>
   </si>
   <si>
+    <t>Term_Deposits_Lists_[WEB]</t>
+  </si>
+  <si>
+    <t>C70772</t>
+  </si>
+  <si>
     <t>Current_Domestic_Accounts-Details-Account_Details_[WEB]</t>
   </si>
   <si>
-    <t>C70772</t>
+    <t>C70773</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Header-Display_[WEB]</t>
   </si>
   <si>
-    <t>C70773</t>
+    <t>C70774</t>
   </si>
   <si>
     <t>Product_Summary-Hide/Show_account_on_Product_List_[WEB]_1</t>
   </si>
   <si>
-    <t>C70774</t>
+    <t>C70775</t>
   </si>
   <si>
     <t>General-Dashboard-Page_overview_[WEB]</t>
   </si>
   <si>
-    <t>C70775</t>
+    <t>C70776</t>
   </si>
   <si>
     <t>Foreign_Current_Account_Product_Details_Account_Details_[WEB]</t>
   </si>
   <si>
-    <t>C70776</t>
+    <t>C70777</t>
   </si>
   <si>
     <t>Current_Accounts-Transactions_Details-Create_Confirmation_[WEB]</t>
   </si>
   <si>
-    <t>C70777</t>
+    <t>C70778</t>
   </si>
   <si>
     <t>Current_Accounts-Transactions_List_select_Currency_[WEB]_2</t>
   </si>
   <si>
-    <t>C70778</t>
+    <t>C70779</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Transactions-Download_option_[WEB]</t>
   </si>
   <si>
-    <t>C70779</t>
+    <t>C70780</t>
   </si>
   <si>
     <t>Foreign_Current_Accounts-Transactions-Filter_By_Type_[WEB]</t>
   </si>
   <si>
-    <t>C70780</t>
+    <t>C70781</t>
   </si>
   <si>
     <t>Current_Domestic_Account-Transactions-Filter_By_Type_[WEB]</t>
   </si>
   <si>
-    <t>C70781</t>
+    <t>C70782</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Transactions-Filter_By_Date-Predefined_Date_Range_[WEB]</t>
   </si>
   <si>
-    <t>C70782</t>
+    <t>C70783</t>
   </si>
   <si>
     <t>Foreign_Current_Accounts-Multiple-Filter_Invalid_[WEB]</t>
   </si>
   <si>
-    <t>C70783</t>
+    <t>C70784</t>
   </si>
   <si>
     <t>Current_Foreign_Accounts-Transactions-Download_option_[WEB]</t>
   </si>
   <si>
-    <t>C70784</t>
+    <t>C70785</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Multiple-Filter_Invalid_[WEB]</t>
   </si>
   <si>
-    <t>C70785</t>
+    <t>C70786</t>
   </si>
   <si>
     <t>Foreign_Current_Account-Transactions-Filter_By_Date-Predefined_Date_Range_[WEB]</t>
   </si>
   <si>
-    <t>C70786</t>
+    <t>C70787</t>
   </si>
   <si>
     <t>Manage_Products-Favorite_account_[WEB]</t>
   </si>
   <si>
-    <t>C70787</t>
+    <t>C70788</t>
   </si>
   <si>
     <t>Manage_Products-Favorite_account-Removal_of_the_favorite_account_[WEB]</t>
   </si>
   <si>
-    <t>C70788</t>
+    <t>C70789</t>
   </si>
   <si>
     <t>Manage_Products-Hide/Show_account_on_Product_List_[WEB]_1</t>
   </si>
   <si>
-    <t>C70789</t>
+    <t>C70790</t>
   </si>
   <si>
     <t>Manage_Products-Hide/Show_account_on_Product_List_Invalid[WEB]_1</t>
   </si>
   <si>
-    <t>C70790</t>
+    <t>C70791</t>
   </si>
   <si>
     <t>Manage_Products-Nickname_Product_Returning_To_Default_Name_[WEB]</t>
   </si>
   <si>
-    <t>C70791</t>
+    <t>C70792</t>
   </si>
   <si>
     <t>Manage_Products-Nickname_Product_[WEB]_Invalid</t>
   </si>
   <si>
-    <t>C70792</t>
+    <t>C70793</t>
   </si>
   <si>
     <t>Manage_Products-Nickname_Product_[WEB]</t>
   </si>
   <si>
-    <t>C70793</t>
+    <t>C70794</t>
   </si>
   <si>
     <t>Products_Current_Accounts-Cheques_[WEB]</t>
   </si>
   <si>
-    <t>C70794</t>
+    <t>C70795</t>
   </si>
   <si>
     <t>Products_Current_Accounts-Cheques-Filter_[WEB]</t>
   </si>
   <si>
-    <t>C70795</t>
+    <t>C70796</t>
   </si>
   <si>
     <t>Products_Current_Accounts-Cheques-Input_Fields-invalid_[WEB]</t>
   </si>
   <si>
-    <t>C70796</t>
+    <t>C70797</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Transactions_List_[WEB]</t>
   </si>
   <si>
-    <t>C70797</t>
+    <t>C70798</t>
   </si>
   <si>
     <t>Current_Foreign_Accounts-Transactions_List_[WEB]</t>
   </si>
   <si>
-    <t>C70798</t>
+    <t>C70799</t>
   </si>
   <si>
     <t>Foreign_Current_Accounts-Transactions_List_select_Currency_[WEB]</t>
   </si>
   <si>
-    <t>C70799</t>
+    <t>C70800</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Details-Financial_Details_[WEB]</t>
   </si>
   <si>
-    <t>C70800</t>
+    <t>C70801</t>
   </si>
   <si>
     <t>Credit_Cards-Header_Display_[WEB]</t>
   </si>
   <si>
-    <t>C70801</t>
+    <t>C70802</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Transactions_List_No_Transactions_[WEB]</t>
   </si>
   <si>
-    <t>C70802</t>
+    <t>C70803</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Transactions_Filter_By_Date-Date_Picker_[WEB]</t>
   </si>
   <si>
-    <t>C70803</t>
+    <t>C70804</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Transactions-Filter_By_Amount_[WEB]</t>
   </si>
   <si>
-    <t>C70804</t>
+    <t>C70805</t>
   </si>
   <si>
     <t>Current_Domestic_Accounts-Transactions-Filter_By_Amount_Invalid_[WEB]</t>
   </si>
   <si>
-    <t>C70805</t>
+    <t>C70806</t>
   </si>
   <si>
     <t>Current_Foreign_Accounts_Product_Details_Financial_Details_Is_Not_Visible_[WEB]</t>
   </si>
   <si>
-    <t>C70806</t>
+    <t>C70807</t>
   </si>
   <si>
     <t>Current_Foreign_Accounts-Transactions_List_No_Transactions_[WEB]</t>
   </si>
   <si>
-    <t>C70807</t>
+    <t>C70808</t>
   </si>
   <si>
     <t>Current_Foreign_Accounts-Transactions_Filter_By_Date-Date_Picker_[WEB]</t>
   </si>
   <si>
-    <t>C70808</t>
+    <t>C70809</t>
   </si>
   <si>
     <t>Current_Foreign_Accounts-Transactions-Filter_By_Amount_[WEB]</t>
   </si>
   <si>
-    <t>C70809</t>
+    <t>C70810</t>
   </si>
   <si>
     <t>Current_Foreign_Accounts-Transactions-Filter_By_Amount_Invalid_[WEB]</t>
   </si>
   <si>
-    <t>C70810</t>
+    <t>C70811</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1032,17 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1305,10 +1321,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -1657,7 +1673,7 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1677,7 +1693,7 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" t="s">
+      <c r="A19" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1757,7 +1773,7 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="4" t="s">
+      <c r="A23" t="s">
         <v>52</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1777,7 +1793,7 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2276,18 +2292,39 @@
         <v>11</v>
       </c>
     </row>
+    <row r="49" spans="1:6">
+      <c r="A49" t="s">
+        <v>104</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F48" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F49" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
-  <conditionalFormatting sqref="A31">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  <conditionalFormatting sqref="A32">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A$1:A$1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B$1:B$1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
credit cards filter by type and amount
</commit_message>
<xml_diff>
--- a/testdata/listForExecution.xlsx
+++ b/testdata/listForExecution.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9467"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="151">
   <si>
     <t>TestName</t>
   </si>
@@ -471,6 +471,18 @@
   </si>
   <si>
     <t>Payments-Domestic_Payments-Back_Button_[WEB]</t>
+  </si>
+  <si>
+    <t>Credit_Cards-Transactions_Filter_By_Type_[WEB]</t>
+  </si>
+  <si>
+    <t>C70830</t>
+  </si>
+  <si>
+    <t>Credit_Cards-Transactions_Filter_By_Amount_[WEB]</t>
+  </si>
+  <si>
+    <t>C70831</t>
   </si>
 </sst>
 </file>
@@ -1434,10 +1446,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -2885,8 +2897,48 @@
         <v>11</v>
       </c>
     </row>
+    <row r="73" spans="1:6">
+      <c r="A73" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F71" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F72" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="A32">
@@ -2913,9 +2965,6 @@
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B72">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A67:A68">
     <cfRule type="duplicateValues" dxfId="0" priority="10"/>
     <cfRule type="duplicateValues" dxfId="0" priority="9"/>
@@ -2926,11 +2975,14 @@
   <conditionalFormatting sqref="B67:B69">
     <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B72:B74">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A1:A65 A69:A70 A73:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="17"/>
     <cfRule type="duplicateValues" dxfId="0" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B51 B73:B1048576">
+  <conditionalFormatting sqref="B1:B51 B75:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="16"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Credit card Transaction details
</commit_message>
<xml_diff>
--- a/testdata/listForExecution.xlsx
+++ b/testdata/listForExecution.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$76</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="156">
   <si>
     <t>TestName</t>
   </si>
@@ -492,6 +492,12 @@
   </si>
   <si>
     <t>C70832</t>
+  </si>
+  <si>
+    <t>Credit_Cards-Transactions_Details[WEB]</t>
+  </si>
+  <si>
+    <t>C70833</t>
   </si>
 </sst>
 </file>
@@ -1455,10 +1461,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
@@ -2986,8 +2992,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F75" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:F76" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="A32">
@@ -3031,14 +3057,14 @@
   <conditionalFormatting sqref="B72:B74">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B75:B76">
+  <conditionalFormatting sqref="B75:B77">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A65 A69:A70 A73:A74 A77:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="20"/>
     <cfRule type="duplicateValues" dxfId="0" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B51 B77:B1048576">
+  <conditionalFormatting sqref="B1:B51 B78:B1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="19"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>